<commit_message>
Code to find occurences of list and enter into spreadsheet
</commit_message>
<xml_diff>
--- a/F_Keywords.xlsx
+++ b/F_Keywords.xlsx
@@ -882,7 +882,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -904,6 +904,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -930,8 +942,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -945,7 +963,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1226,8 +1250,8 @@
   </sheetPr>
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>